<commit_message>
Tweek to home page and uploading updated subject names
</commit_message>
<xml_diff>
--- a/Data/CourseNames(Revised).xlsx
+++ b/Data/CourseNames(Revised).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FCE593A-EE54-4758-B708-E6B0033314AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DFDEA88-E727-4A8D-8543-0B9EA93E2452}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{B49CE345-F9AB-4D69-A0EE-F398744FB770}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="86">
   <si>
     <t>Geometry A</t>
   </si>
   <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
     <t>English 3 A</t>
   </si>
   <si>
@@ -267,13 +264,25 @@
     <t>CreditHours</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
     <t>Elective</t>
   </si>
   <si>
     <t>History</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Practical Arts</t>
+  </si>
+  <si>
+    <t>Personal Finance</t>
+  </si>
+  <si>
+    <t>Fine Arts</t>
   </si>
 </sst>
 </file>
@@ -627,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE9C14C-2F35-402F-8E90-C477E078AF1C}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,16 +650,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>78</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -658,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>200</v>
@@ -669,13 +678,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -683,10 +692,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
       <c r="C4">
         <v>300</v>
@@ -697,13 +706,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -711,10 +720,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
       <c r="C6">
         <v>200</v>
@@ -725,13 +734,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>0.5</v>
@@ -739,13 +748,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>0.5</v>
@@ -753,10 +762,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -767,13 +776,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>0.5</v>
@@ -781,13 +790,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>0.5</v>
@@ -795,13 +804,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>0.5</v>
@@ -809,13 +818,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>0.5</v>
@@ -823,10 +832,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -837,13 +846,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>0.5</v>
@@ -851,13 +860,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>0.5</v>
@@ -865,13 +874,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>0.5</v>
@@ -879,10 +888,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>300</v>
@@ -893,13 +902,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19">
         <v>0.5</v>
@@ -907,13 +916,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <v>0.5</v>
@@ -921,13 +930,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <v>0.5</v>
@@ -935,10 +944,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>100</v>
@@ -949,13 +958,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <v>0.5</v>
@@ -963,13 +972,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>0.5</v>
@@ -977,13 +986,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25">
         <v>0.5</v>
@@ -991,13 +1000,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <v>0.5</v>
@@ -1005,13 +1014,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27">
         <v>0.5</v>
@@ -1019,13 +1028,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28">
         <v>0.5</v>
@@ -1033,13 +1042,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29">
         <v>0.5</v>
@@ -1047,13 +1056,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30">
         <v>0.5</v>
@@ -1061,13 +1070,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31">
         <v>0.5</v>
@@ -1075,13 +1084,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32">
         <v>0.5</v>
@@ -1089,13 +1098,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33">
         <v>0.5</v>
@@ -1103,13 +1112,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
         <v>0.5</v>
@@ -1117,13 +1126,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35">
         <v>0.5</v>
@@ -1131,13 +1140,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36">
         <v>0.5</v>
@@ -1145,13 +1154,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37">
         <v>0.5</v>
@@ -1159,10 +1168,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C38">
         <v>200</v>
@@ -1173,13 +1182,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39">
         <v>0.5</v>
@@ -1187,10 +1196,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40">
         <v>200</v>
@@ -1201,13 +1210,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41">
         <v>0.5</v>
@@ -1215,10 +1224,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>300</v>
@@ -1229,13 +1238,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43">
         <v>0.5</v>
@@ -1243,13 +1252,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44">
         <v>0.5</v>
@@ -1257,10 +1266,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1271,13 +1280,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46">
         <v>0.5</v>
@@ -1285,13 +1294,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47">
         <v>0.5</v>
@@ -1299,13 +1308,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48">
         <v>0.5</v>
@@ -1313,13 +1322,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49">
         <v>0.5</v>
@@ -1327,13 +1336,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50">
         <v>0.5</v>
@@ -1341,10 +1350,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1355,13 +1364,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52">
         <v>0.5</v>
@@ -1369,13 +1378,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53">
         <v>0.5</v>
@@ -1383,10 +1392,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54">
         <v>300</v>
@@ -1397,13 +1406,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D55">
         <v>0.5</v>
@@ -1411,10 +1420,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56">
         <v>100</v>
@@ -1425,13 +1434,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57">
         <v>0.5</v>
@@ -1439,13 +1448,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58">
         <v>0.5</v>
@@ -1453,13 +1462,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59">
         <v>0.5</v>
@@ -1467,10 +1476,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" t="s">
         <v>63</v>
-      </c>
-      <c r="B60" t="s">
-        <v>64</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1481,13 +1490,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D61">
         <v>0.5</v>
@@ -1495,13 +1504,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62">
         <v>0.5</v>
@@ -1509,13 +1518,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63">
         <v>0.5</v>
@@ -1523,13 +1532,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D64">
         <v>0.5</v>
@@ -1537,13 +1546,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D65">
         <v>0.5</v>
@@ -1551,13 +1560,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D66">
         <v>0.5</v>
@@ -1565,13 +1574,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67">
         <v>0.5</v>
@@ -1579,13 +1588,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D68">
         <v>0.5</v>
@@ -1593,13 +1602,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D69">
         <v>0.5</v>
@@ -1607,13 +1616,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D70">
         <v>0.5</v>
@@ -1621,13 +1630,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D71">
         <v>0.5</v>

</xml_diff>